<commit_message>
Set print formatting on each tab
</commit_message>
<xml_diff>
--- a/Template/RollVoltab6.xlsx
+++ b/Template/RollVoltab6.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\psg-prog\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1869369-7445-42CD-8753-4C40A2430729}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,7 +184,7 @@
     <definedName name="Volume8" localSheetId="7">Route8!$M$3:$M$5</definedName>
     <definedName name="Volume9" localSheetId="8">Route9!$M$3:$M$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -901,13 +902,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup fitToHeight="16" orientation="landscape" r:id="rId1"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -1060,12 +1063,16 @@
       <c r="O6" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="91" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -1213,12 +1220,16 @@
       <c r="O6" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="97" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
@@ -1366,7 +1377,8 @@
       <c r="O6" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="97" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1549,18 +1561,20 @@
       <c r="O7" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="94" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="70" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr codeName="Sheet4"/>
+  <sheetPr codeName="Sheet4">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="M2:N2"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,13 +1728,16 @@
       <c r="O6" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="71" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr codeName="Sheet5"/>
+  <sheetPr codeName="Sheet5">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView zoomScale="106" workbookViewId="0">
@@ -1878,13 +1895,16 @@
       <c r="O6" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="70" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr codeName="Sheet6"/>
+  <sheetPr codeName="Sheet6">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2035,13 +2055,16 @@
       <c r="O6" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr codeName="Sheet7"/>
+  <sheetPr codeName="Sheet7">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2192,13 +2215,16 @@
       <c r="O6" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr codeName="Sheet8"/>
+  <sheetPr codeName="Sheet8">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2349,14 +2375,16 @@
       <c r="O6" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr codeName="Sheet9"/>
+  <sheetPr codeName="Sheet9">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2507,13 +2535,16 @@
       <c r="O6" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr codeName="Sheet10"/>
+  <sheetPr codeName="Sheet10">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2664,6 +2695,7 @@
       <c r="O6" s="11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>